<commit_message>
new orders are sent as an email to admin
</commit_message>
<xml_diff>
--- a/order_forms/current_order_nj.xlsx
+++ b/order_forms/current_order_nj.xlsx
@@ -1170,9 +1170,7 @@
       <c r="Q10" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="R10" s="29">
-        <v>4</v>
-      </c>
+      <c r="R10" s="29"/>
       <c r="S10" s="26"/>
       <c r="T10" s="25"/>
       <c r="U10" s="26"/>

</xml_diff>